<commit_message>
2021 F1040 Schedule 2
</commit_message>
<xml_diff>
--- a/Federal/f1040s1-2021.xlsx
+++ b/Federal/f1040s1-2021.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
-    <t>Form 1040 SCHEDULE 1    Additional Income and Adjustments to Income     2019</t>
-  </si>
-  <si>
     <t>Part I Additional Income</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>Taxable refunds, credits, or offsets of state and local income taxes</t>
+  </si>
+  <si>
+    <t>Form 1040 SCHEDULE 1    Additional Income and Adjustments to Income     2021</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1059,6 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1069,10 +1068,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1083,12 +1079,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1101,10 +1091,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1431,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1444,828 +1444,839 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="5" t="s">
+      <c r="B4" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="B9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="C12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="C13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="C14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="C15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="C17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="C18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="C20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="C21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="C22" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="C23" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="C24" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="C25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="C26" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="C27" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="17"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="29" t="s">
+      <c r="B29" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="22">
+      <c r="F29" s="18">
         <f>SUM(D12:D28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="24">
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="20">
         <f>SUM(F3:F29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="B34" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B35" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="B36" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="B37" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="B38" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="B39" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="B40" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="B41" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="B42" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="B43" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+      <c r="B44" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="15"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="B46" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="C46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="17"/>
-    </row>
-    <row r="47" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="B47" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="C47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="19"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="17"/>
-    </row>
-    <row r="48" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="B48" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="C48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="17"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="B49" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="C49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="17"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="B50" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="C50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="17"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="B51" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="C51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="19"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="17"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="B52" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="19"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="17"/>
-    </row>
-    <row r="53" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="B53" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="C53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="19"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="17"/>
-    </row>
-    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="B54" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="C54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="19"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="17"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="B55" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="C55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="19"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D55" s="23"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="17"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="B56" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="C56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="17"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="B57" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="C57" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="19"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D57" s="23"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="17"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="B58" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F58" s="22">
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="18">
         <f>SUM(D46:D57)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F59" s="24">
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" s="20">
         <f>SUM(F32:F58)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
@@ -2273,22 +2284,11 @@
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="B58:D58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>